<commit_message>
studen eingetragen - loh
</commit_message>
<xml_diff>
--- a/Protokolle/Stundentafel.xlsx
+++ b/Protokolle/Stundentafel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19222"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dokumente\[Meine Dokumente]\[Schule]\FH\[Lehrveranstaltungen]\WS1\ITP\FHTW Robotics Challenge 2018\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Eigene Dokumente\[Meine Dokumente]\[Schule]\FH\[Lehrveranstaltungen]\SS18\ITPS\Alexa &amp; LEGO\ITP-Alexa-Pen\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="103" documentId="06DCE2DC504AABB48E557451A2596931409E6D38" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{C551DC3D-0A7A-46A4-A54A-5505F6246D00}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{3AEA8729-1D2D-4DDD-BC54-213FC074B6FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loh" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="8">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="10">
   <si>
     <t>Protokoll - LOH</t>
   </si>
@@ -53,12 +53,18 @@
   <si>
     <t>Protokoll - Klaassen</t>
   </si>
+  <si>
+    <t>Erste Besprechung und Plaung</t>
+  </si>
+  <si>
+    <t>Einlesung in die Programmierung von Alexa und Installation des Programms für EV3</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -600,7 +606,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="56">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -748,6 +754,9 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -768,7 +777,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1066,11 +1075,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
-      <selection activeCell="F17" sqref="F17"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
@@ -1079,13 +1088,13 @@
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="4" spans="2:4" ht="35.25" customHeight="1">
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
@@ -1096,109 +1105,117 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
         <v>12</v>
       </c>
-      <c r="C6" s="7"/>
-      <c r="D6" s="15"/>
-    </row>
-    <row r="7" spans="2:4">
+      <c r="C6" s="31" t="s">
+        <v>8</v>
+      </c>
+      <c r="D6" s="15">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="7" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>13</v>
       </c>
-      <c r="C7" s="16"/>
-      <c r="D7" s="11"/>
-    </row>
-    <row r="8" spans="2:4">
+      <c r="C7" s="16" t="s">
+        <v>9</v>
+      </c>
+      <c r="D7" s="55">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>14</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="15"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>15</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>16</v>
       </c>
       <c r="C10" s="16"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>17</v>
       </c>
       <c r="C11" s="31"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="32">
         <v>18</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="33"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="32">
         <v>19</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="33"/>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>20</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>21</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>22</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>23</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="9">
         <v>24</v>
       </c>
       <c r="C18" s="36"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" s="37" t="s">
         <v>4</v>
       </c>
       <c r="D23" s="38">
-        <f>SUM(D6:D21)</f>
-        <v>0</v>
+        <f>SUM(D6:D18)</f>
+        <v>5.5</v>
       </c>
     </row>
   </sheetData>
@@ -1211,30 +1228,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08664FD9-0ED2-4C12-9011-D42332A3AFEC}">
   <dimension ref="B3:D19"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{A7DEBC2E-57E9-5E84-AEB4-F569604DC6BC}">
+    <sheetView workbookViewId="0">
       <selection activeCell="G20" sqref="G20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>5</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1245,96 +1262,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="42"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>12</v>
       </c>
       <c r="C7" s="41"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>13</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>14</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>15</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>16</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>17</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>18</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>19</v>
       </c>
       <c r="C14" s="7"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>20</v>
       </c>
       <c r="C15" s="7"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>21</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>22</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
         <v>23</v>
       </c>
       <c r="C18" s="7"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
         <v>24</v>
       </c>
@@ -1350,30 +1367,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="F19" sqref="F19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.85546875" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>6</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
@@ -1384,103 +1401,103 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="20"/>
       <c r="C6" s="4"/>
       <c r="D6" s="21"/>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="22">
         <v>12</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="23"/>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="22">
         <v>13</v>
       </c>
       <c r="C8" s="16"/>
       <c r="D8" s="24"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="22">
         <v>14</v>
       </c>
       <c r="C9" s="16"/>
       <c r="D9" s="25"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="22">
         <v>15</v>
       </c>
       <c r="C10" s="10"/>
       <c r="D10" s="25"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="22">
         <v>16</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="25"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="22">
         <v>17</v>
       </c>
       <c r="C12" s="44"/>
       <c r="D12" s="25"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="22">
         <v>18</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="27"/>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="45">
         <v>19</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="25"/>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="22">
         <v>20</v>
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="46"/>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="22">
         <v>21</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="22">
         <v>22</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="26">
         <v>23</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="28">
         <v>24</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="47"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="37" t="s">
         <v>4</v>
       </c>
@@ -1498,30 +1515,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>7</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="45">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1532,96 +1549,96 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="6">
         <v>12</v>
       </c>
       <c r="C7" s="7"/>
       <c r="D7" s="15"/>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="6">
         <v>13</v>
       </c>
       <c r="C8" s="10"/>
       <c r="D8" s="11"/>
     </row>
-    <row r="9" spans="2:4">
+    <row r="9" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B9" s="6">
         <v>14</v>
       </c>
       <c r="C9" s="7"/>
       <c r="D9" s="8"/>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
         <v>15</v>
       </c>
       <c r="C10" s="7"/>
       <c r="D10" s="8"/>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
         <v>16</v>
       </c>
       <c r="C11" s="7"/>
       <c r="D11" s="8"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>17</v>
       </c>
       <c r="C12" s="7"/>
       <c r="D12" s="8"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
         <v>18</v>
       </c>
       <c r="C13" s="7"/>
       <c r="D13" s="8"/>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
         <v>19</v>
       </c>
       <c r="C14" s="53"/>
       <c r="D14" s="54"/>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
         <v>20</v>
       </c>
       <c r="C15" s="10"/>
       <c r="D15" s="11"/>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
         <v>21</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="11"/>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
         <v>22</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="11"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="32">
         <v>23</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="52"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="50">
         <v>24</v>
       </c>

</xml_diff>

<commit_message>
aws doku, stunden update
</commit_message>
<xml_diff>
--- a/Protokolle/Stundentafel.xlsx
+++ b/Protokolle/Stundentafel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\OneDrive - FH Technikum Wien\2SEM\ITP-Alexa-Pen\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B7A1F9FC-8A06-42F6-808D-4F796A189EC8}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{49AD2868-5341-4A23-8EAE-624854E0D1FE}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="22">
   <si>
     <t>Protokoll - LOH</t>
   </si>
@@ -91,6 +91,9 @@
   </si>
   <si>
     <t>Erweiterung AWS und Amazon Dev nach Anleitung</t>
+  </si>
+  <si>
+    <t>Dokumentation AWS</t>
   </si>
 </sst>
 </file>
@@ -1267,7 +1270,7 @@
   <dimension ref="B3:D23"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1357,15 +1360,19 @@
         <v>20</v>
       </c>
       <c r="D11" s="8">
-        <v>1.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
         <v>17</v>
       </c>
-      <c r="C12" s="16"/>
-      <c r="D12" s="8"/>
+      <c r="C12" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" s="8">
+        <v>4</v>
+      </c>
     </row>
     <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
@@ -1422,7 +1429,7 @@
       </c>
       <c r="D23" s="38">
         <f>SUM(D7:D21)</f>
-        <v>8.5</v>
+        <v>14.5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Alles ist noch im Arsch
Internetanbindung noch nicht möglich!
RobotC läuft wieder. Jedoch ist eine Internetanbindung unmöglich.
EV3-dev funkt nur sporadisch. Internet Sharing über USB oder Bluetooth funkt nicht. Kommunikation über SSH möglich.
</commit_message>
<xml_diff>
--- a/Protokolle/Stundentafel.xlsx
+++ b/Protokolle/Stundentafel.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benni\OneDrive - FH Technikum Wien\BIF 2\ITPS - IT Projektarbeit 2\ITP-Alexa-Pen\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="6" documentId="6_{07966A21-D58C-4113-B183-F3A4EF288D1E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{6834E6E7-8107-42A8-BA23-88F514E65183}"/>
+  <xr:revisionPtr revIDLastSave="19" documentId="6_{07966A21-D58C-4113-B183-F3A4EF288D1E}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{A44B93A7-8A34-4FFA-8112-0D950D5A80A1}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="32">
   <si>
     <t>Protokoll - LOH</t>
   </si>
@@ -105,9 +105,6 @@
     <t>Recherche AWS, Konstruktion</t>
   </si>
   <si>
-    <t>3</t>
-  </si>
-  <si>
     <t>Besprechung zur Implementierung v. Skills</t>
   </si>
   <si>
@@ -126,7 +123,7 @@
     <t>Peer Review + EV3-Dev installation</t>
   </si>
   <si>
-    <t>EV3-Dev Troubleshooting</t>
+    <t>EV3-Dev + RobotC Troubleshooting</t>
   </si>
 </sst>
 </file>
@@ -675,7 +672,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="59">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -813,17 +810,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="49" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="28" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="35" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="6" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="2" fillId="0" borderId="8" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="25" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="1" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1420,7 +1427,7 @@
         <v>18</v>
       </c>
       <c r="C13" s="16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="8">
         <v>1</v>
@@ -1654,8 +1661,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1691,7 +1698,7 @@
     <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
-      <c r="D6" s="5"/>
+      <c r="D6" s="54"/>
     </row>
     <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
@@ -1700,7 +1707,7 @@
       <c r="C7" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D7" s="15">
+      <c r="D7" s="55">
         <v>2</v>
       </c>
     </row>
@@ -1711,8 +1718,8 @@
       <c r="C8" s="16" t="s">
         <v>24</v>
       </c>
-      <c r="D8" s="11" t="s">
-        <v>25</v>
+      <c r="D8" s="52">
+        <v>3</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="29" x14ac:dyDescent="0.35">
@@ -1720,9 +1727,9 @@
         <v>14</v>
       </c>
       <c r="C9" s="10" t="s">
-        <v>26</v>
-      </c>
-      <c r="D9" s="8">
+        <v>25</v>
+      </c>
+      <c r="D9" s="56">
         <v>2</v>
       </c>
     </row>
@@ -1731,9 +1738,9 @@
         <v>15</v>
       </c>
       <c r="C10" s="7" t="s">
-        <v>27</v>
-      </c>
-      <c r="D10" s="8">
+        <v>26</v>
+      </c>
+      <c r="D10" s="56">
         <v>3</v>
       </c>
     </row>
@@ -1742,9 +1749,9 @@
         <v>16</v>
       </c>
       <c r="C11" s="7" t="s">
-        <v>28</v>
-      </c>
-      <c r="D11" s="8">
+        <v>27</v>
+      </c>
+      <c r="D11" s="56">
         <v>2</v>
       </c>
     </row>
@@ -1753,9 +1760,9 @@
         <v>17</v>
       </c>
       <c r="C12" s="7" t="s">
-        <v>29</v>
-      </c>
-      <c r="D12" s="8">
+        <v>28</v>
+      </c>
+      <c r="D12" s="56">
         <v>2</v>
       </c>
     </row>
@@ -1764,9 +1771,9 @@
         <v>18</v>
       </c>
       <c r="C13" s="31" t="s">
-        <v>31</v>
-      </c>
-      <c r="D13" s="8">
+        <v>30</v>
+      </c>
+      <c r="D13" s="56">
         <v>5</v>
       </c>
     </row>
@@ -1774,11 +1781,11 @@
       <c r="B14" s="6">
         <v>19</v>
       </c>
-      <c r="C14" s="54" t="s">
-        <v>32</v>
-      </c>
-      <c r="D14" s="53" t="s">
-        <v>25</v>
+      <c r="C14" s="51" t="s">
+        <v>31</v>
+      </c>
+      <c r="D14" s="53">
+        <v>5</v>
       </c>
     </row>
     <row r="15" spans="2:4" x14ac:dyDescent="0.35">
@@ -1786,35 +1793,35 @@
         <v>20</v>
       </c>
       <c r="C15" s="10"/>
-      <c r="D15" s="11"/>
+      <c r="D15" s="55"/>
     </row>
     <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>21</v>
       </c>
       <c r="C16" s="10"/>
-      <c r="D16" s="11"/>
+      <c r="D16" s="55"/>
     </row>
     <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>22</v>
       </c>
       <c r="C17" s="10"/>
-      <c r="D17" s="11"/>
+      <c r="D17" s="55"/>
     </row>
     <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="32">
         <v>23</v>
       </c>
       <c r="C18" s="30"/>
-      <c r="D18" s="52"/>
+      <c r="D18" s="57"/>
     </row>
     <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="50">
         <v>24</v>
       </c>
       <c r="C19" s="43"/>
-      <c r="D19" s="51"/>
+      <c r="D19" s="58"/>
     </row>
     <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
@@ -1822,7 +1829,7 @@
       </c>
       <c r="D23">
         <f>SUM(D6:D21)</f>
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Dokumenation C# .net anbindung
</commit_message>
<xml_diff>
--- a/Protokolle/Stundentafel.xlsx
+++ b/Protokolle/Stundentafel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19226"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\OneDrive - FH Technikum Wien\2SEM\ITP-Alexa-Pen\Protokolle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Benni\OneDrive - FH Technikum Wien\BIF 2\ITPS - IT Projektarbeit 2\ITP-Alexa-Pen\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{BB182BD3-D0BB-45E1-ACF3-9C4BE49B3AE0}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="2" documentId="6_{8E273E19-A6BB-4FE6-9E49-C223C21CB824}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="33" xr10:uidLastSave="{A24B9BC7-7ECC-4C18-B1F5-5B171547393E}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loh" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="50" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="34">
   <si>
     <t>Protokoll - LOH</t>
   </si>
@@ -127,6 +127,9 @@
   </si>
   <si>
     <t>SNS / SQS (Amazon Message-Queue Services) Einrichten, Troubleshooting C#-Desktop-Anwendung zur Nachrichtenübertragung an EV3, Bluetooth-EV3 Troubleshooting</t>
+  </si>
+  <si>
+    <t>C#-Desktop-Anwendung zur Nachrichtenübertragung an EV3 einrichten, Bluetooth-EV3 Troubleshooting, Dokumentation</t>
   </si>
 </sst>
 </file>
@@ -837,7 +840,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Standard" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -853,7 +856,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1155,22 +1158,22 @@
       <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="11.453125" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="11.42578125" style="1"/>
+    <col min="1" max="1" width="11.453125" style="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
-    <col min="3" max="3" width="37.85546875" style="1" customWidth="1"/>
-    <col min="4" max="4" width="15.85546875" style="1" customWidth="1"/>
-    <col min="5" max="16384" width="11.42578125" style="1"/>
+    <col min="3" max="3" width="37.81640625" style="1" customWidth="1"/>
+    <col min="4" max="4" width="15.81640625" style="1" customWidth="1"/>
+    <col min="5" max="16384" width="11.453125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="4" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="4" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="B4" s="12" t="s">
         <v>1</v>
       </c>
@@ -1181,12 +1184,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B5" s="3"/>
       <c r="C5" s="4"/>
       <c r="D5" s="5"/>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="6">
         <v>12</v>
       </c>
@@ -1197,7 +1200,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
         <v>13</v>
       </c>
@@ -1208,7 +1211,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B8" s="6">
         <v>14</v>
       </c>
@@ -1219,7 +1222,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>15</v>
       </c>
@@ -1230,7 +1233,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>16</v>
       </c>
@@ -1241,7 +1244,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>17</v>
       </c>
@@ -1252,56 +1255,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="32">
         <v>18</v>
       </c>
       <c r="C12" s="34"/>
       <c r="D12" s="33"/>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="32">
         <v>19</v>
       </c>
       <c r="C13" s="34"/>
       <c r="D13" s="33"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="6">
         <v>20</v>
       </c>
       <c r="C14" s="16"/>
       <c r="D14" s="15"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>21</v>
       </c>
       <c r="C15" s="16"/>
       <c r="D15" s="8"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>22</v>
       </c>
       <c r="C16" s="16"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>23</v>
       </c>
       <c r="C17" s="16"/>
       <c r="D17" s="15"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="9">
         <v>24</v>
       </c>
       <c r="C18" s="36"/>
       <c r="D18" s="35"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C23" s="37" t="s">
         <v>11</v>
       </c>
@@ -1320,30 +1323,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08664FD9-0ED2-4C12-9011-D42332A3AFEC}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
-      <selection activeCell="E18" sqref="E18"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="C15" sqref="C15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.26953125" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>12</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1354,12 +1357,12 @@
         <v>13</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="42"/>
       <c r="D6" s="5"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
         <v>12</v>
       </c>
@@ -1370,7 +1373,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="6">
         <v>13</v>
       </c>
@@ -1381,7 +1384,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>14</v>
       </c>
@@ -1392,7 +1395,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>15</v>
       </c>
@@ -1403,7 +1406,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>16</v>
       </c>
@@ -1414,7 +1417,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="6">
         <v>17</v>
       </c>
@@ -1425,7 +1428,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>18</v>
       </c>
@@ -1436,14 +1439,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="6">
         <v>19</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="8"/>
     </row>
-    <row r="15" spans="2:4" ht="75" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="72.5" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>20</v>
       </c>
@@ -1454,35 +1457,35 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>21</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="8"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>22</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="8"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="6">
         <v>23</v>
       </c>
       <c r="C18" s="10"/>
       <c r="D18" s="8"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="6">
         <v>24</v>
       </c>
       <c r="C19" s="10"/>
       <c r="D19" s="8"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C23" s="37" t="s">
         <v>11</v>
       </c>
@@ -1504,26 +1507,26 @@
       <selection activeCell="D11" sqref="D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="14.85546875" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.140625" customWidth="1"/>
+    <col min="2" max="2" width="14.81640625" customWidth="1"/>
+    <col min="3" max="3" width="36.26953125" customWidth="1"/>
+    <col min="4" max="4" width="17.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>18</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="17" t="s">
         <v>1</v>
       </c>
@@ -1534,12 +1537,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="20"/>
       <c r="C6" s="4"/>
       <c r="D6" s="21"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="22">
         <v>12</v>
       </c>
@@ -1550,7 +1553,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="22">
         <v>13</v>
       </c>
@@ -1561,7 +1564,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B9" s="22">
         <v>14</v>
       </c>
@@ -1572,7 +1575,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" ht="43.5" x14ac:dyDescent="0.35">
       <c r="B10" s="22">
         <v>15</v>
       </c>
@@ -1583,14 +1586,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="22">
         <v>16</v>
       </c>
       <c r="C11" s="10"/>
       <c r="D11" s="25"/>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="22">
         <v>17</v>
       </c>
@@ -1601,56 +1604,56 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="22">
         <v>18</v>
       </c>
       <c r="C13" s="30"/>
       <c r="D13" s="27"/>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="45">
         <v>19</v>
       </c>
       <c r="C14" s="10"/>
       <c r="D14" s="25"/>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B15" s="22">
         <v>20</v>
       </c>
       <c r="C15" s="41"/>
       <c r="D15" s="46"/>
     </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="22">
         <v>21</v>
       </c>
       <c r="C16" s="7"/>
       <c r="D16" s="23"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="22">
         <v>22</v>
       </c>
       <c r="C17" s="7"/>
       <c r="D17" s="23"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="26">
         <v>23</v>
       </c>
       <c r="C18" s="48"/>
       <c r="D18" s="49"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="28">
         <v>24</v>
       </c>
       <c r="C19" s="29"/>
       <c r="D19" s="47"/>
     </row>
-    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C24" s="37" t="s">
         <v>11</v>
       </c>
@@ -1668,30 +1671,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F15" sqref="F15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="13.7109375" customWidth="1"/>
+    <col min="2" max="2" width="13.7265625" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>23</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B5" s="12" t="s">
         <v>1</v>
       </c>
@@ -1702,12 +1705,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B6" s="3"/>
       <c r="C6" s="4"/>
       <c r="D6" s="54"/>
     </row>
-    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B7" s="6">
         <v>12</v>
       </c>
@@ -1718,7 +1721,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B8" s="6">
         <v>13</v>
       </c>
@@ -1729,7 +1732,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:4" ht="29" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
         <v>14</v>
       </c>
@@ -1740,7 +1743,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B10" s="6">
         <v>15</v>
       </c>
@@ -1751,7 +1754,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B11" s="6">
         <v>16</v>
       </c>
@@ -1762,7 +1765,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B12" s="6">
         <v>17</v>
       </c>
@@ -1773,7 +1776,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B13" s="6">
         <v>18</v>
       </c>
@@ -1784,7 +1787,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B14" s="6">
         <v>19</v>
       </c>
@@ -1795,48 +1798,52 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:4" ht="58" x14ac:dyDescent="0.35">
       <c r="B15" s="6">
         <v>20</v>
       </c>
-      <c r="C15" s="10"/>
-      <c r="D15" s="55"/>
-    </row>
-    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
+      <c r="C15" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="D15" s="55">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="16" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B16" s="6">
         <v>21</v>
       </c>
       <c r="C16" s="10"/>
       <c r="D16" s="55"/>
     </row>
-    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B17" s="6">
         <v>22</v>
       </c>
       <c r="C17" s="10"/>
       <c r="D17" s="55"/>
     </row>
-    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B18" s="32">
         <v>23</v>
       </c>
       <c r="C18" s="30"/>
       <c r="D18" s="57"/>
     </row>
-    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.35">
       <c r="B19" s="50">
         <v>24</v>
       </c>
       <c r="C19" s="43"/>
       <c r="D19" s="58"/>
     </row>
-    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.35">
       <c r="C23" t="s">
         <v>11</v>
       </c>
       <c r="D23">
         <f>SUM(D6:D21)</f>
-        <v>24</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Stundentafel + Erweiterung "Anleitung C#-Desktopapplikation"
</commit_message>
<xml_diff>
--- a/Protokolle/Stundentafel.xlsx
+++ b/Protokolle/Stundentafel.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="19330"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\dditt\OneDrive - FH Technikum Wien\2SEM\ITP-Alexa-Pen\Protokolle\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\David\OneDrive - FH Technikum Wien\2SEM\ITP-Alexa-Pen\Protokolle\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="5_{80085711-82B1-4FEA-B396-94E013093121}" xr6:coauthVersionLast="34" xr6:coauthVersionMax="34" xr10:uidLastSave="{2E4E26C2-2991-4925-85A8-4415CBD7D48B}"/>
+  <xr:revisionPtr revIDLastSave="11" documentId="5_{80085711-82B1-4FEA-B396-94E013093121}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="34" xr10:uidLastSave="{C7FBFDC3-8809-42F1-84EA-285FF271315B}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" firstSheet="3" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="11610" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Loh" sheetId="1" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="60" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="62" uniqueCount="42">
   <si>
     <t>Protokoll - LOH</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>C#-Anwendung erweitert, Präsentationsvorbereitung und Dokumentierabsprache</t>
+  </si>
+  <si>
+    <t>Fertigstellung der Dokumentation</t>
   </si>
 </sst>
 </file>
@@ -161,7 +164,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
-  <fonts count="6">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -703,7 +706,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="57">
+  <cellXfs count="58">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -856,6 +859,9 @@
     </xf>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="34" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -875,7 +881,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1173,11 +1179,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:D23"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0" xr3:uid="{AEA406A1-0E4B-5B11-9CD5-51D6E497D94C}">
+    <sheetView topLeftCell="A13" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.42578125" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="11.42578125" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="11.42578125" style="1"/>
     <col min="2" max="2" width="17" style="1" customWidth="1"/>
@@ -1186,13 +1192,13 @@
     <col min="5" max="16384" width="11.42578125" style="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:4">
+    <row r="2" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C2" s="2" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="2:4" ht="15.75" thickBot="1"/>
-    <row r="4" spans="2:4" ht="35.25" customHeight="1">
+    <row r="3" spans="2:4" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="4" spans="2:4" ht="35.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" s="11" t="s">
         <v>1</v>
       </c>
@@ -1203,11 +1209,11 @@
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="2:4">
+    <row r="5" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B5" s="3"/>
       <c r="D5" s="4"/>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="5">
         <v>12</v>
       </c>
@@ -1218,7 +1224,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>13</v>
       </c>
@@ -1229,7 +1235,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="2:4" ht="30">
+    <row r="8" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>14</v>
       </c>
@@ -1240,7 +1246,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30">
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>15</v>
       </c>
@@ -1251,7 +1257,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30">
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>16</v>
       </c>
@@ -1262,7 +1268,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>17</v>
       </c>
@@ -1273,21 +1279,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="31">
         <v>18</v>
       </c>
       <c r="C12" s="33"/>
       <c r="D12" s="32"/>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="31">
         <v>19</v>
       </c>
       <c r="C13" s="33"/>
       <c r="D13" s="32"/>
     </row>
-    <row r="14" spans="2:4" ht="60">
+    <row r="14" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>20</v>
       </c>
@@ -1298,7 +1304,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:4">
+    <row r="15" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>21</v>
       </c>
@@ -1309,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="69" customHeight="1">
+    <row r="16" spans="2:4" ht="69" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>22</v>
       </c>
@@ -1320,21 +1326,21 @@
         <v>5.5</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>23</v>
       </c>
       <c r="C17" s="15"/>
       <c r="D17" s="14"/>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="8">
         <v>24</v>
       </c>
       <c r="C18" s="35"/>
       <c r="D18" s="34"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" s="36" t="s">
         <v>14</v>
       </c>
@@ -1353,30 +1359,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{08664FD9-0ED2-4C12-9011-D42332A3AFEC}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0" xr3:uid="{A7DEBC2E-57E9-5E84-AEB4-F569604DC6BC}">
-      <selection activeCell="E16" sqref="E16"/>
+    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>15</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1387,12 +1393,12 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="40"/>
       <c r="D6" s="4"/>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>12</v>
       </c>
@@ -1403,7 +1409,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>13</v>
       </c>
@@ -1414,7 +1420,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30">
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>14</v>
       </c>
@@ -1425,7 +1431,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="30">
+    <row r="10" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>15</v>
       </c>
@@ -1436,7 +1442,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="2:4" ht="30">
+    <row r="11" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>16</v>
       </c>
@@ -1447,7 +1453,7 @@
         <v>3.5</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>17</v>
       </c>
@@ -1458,7 +1464,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>18</v>
       </c>
@@ -1469,14 +1475,14 @@
         <v>1</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>19</v>
       </c>
       <c r="C14" s="9"/>
       <c r="D14" s="7"/>
     </row>
-    <row r="15" spans="2:4" ht="150">
+    <row r="15" spans="2:4" ht="150" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>20</v>
       </c>
@@ -1487,7 +1493,7 @@
         <v>7</v>
       </c>
     </row>
-    <row r="16" spans="2:4" ht="30">
+    <row r="16" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>21</v>
       </c>
@@ -1498,34 +1504,42 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="17" spans="2:4">
+    <row r="17" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
-        <v>22</v>
-      </c>
-      <c r="C17" s="9"/>
-      <c r="D17" s="7"/>
-    </row>
-    <row r="18" spans="2:4">
+        <v>23</v>
+      </c>
+      <c r="C17" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="D17" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="5">
-        <v>23</v>
-      </c>
-      <c r="C18" s="9"/>
-      <c r="D18" s="7"/>
-    </row>
-    <row r="19" spans="2:4">
+        <v>26</v>
+      </c>
+      <c r="C18" s="57" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="7">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="5">
         <v>24</v>
       </c>
       <c r="C19" s="9"/>
       <c r="D19" s="7"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" s="36" t="s">
         <v>14</v>
       </c>
       <c r="D23" s="37">
         <f>SUM(D7:D21)</f>
-        <v>25</v>
+        <v>29</v>
       </c>
     </row>
   </sheetData>
@@ -1537,30 +1551,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="B3:D24"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0" xr3:uid="{958C4451-9541-5A59-BF78-D2F731DF1C81}">
+    <sheetView topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="D15" sqref="D15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="14.7109375" customWidth="1"/>
     <col min="3" max="3" width="36.28515625" customWidth="1"/>
     <col min="4" max="4" width="17.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>24</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="16" t="s">
         <v>1</v>
       </c>
@@ -1571,12 +1585,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="19"/>
       <c r="C6" s="1"/>
       <c r="D6" s="20"/>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="21">
         <v>12</v>
       </c>
@@ -1587,7 +1601,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="21">
         <v>13</v>
       </c>
@@ -1598,7 +1612,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="45">
+    <row r="9" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B9" s="21">
         <v>14</v>
       </c>
@@ -1609,7 +1623,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="2:4" ht="45">
+    <row r="10" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B10" s="21">
         <v>15</v>
       </c>
@@ -1620,14 +1634,14 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="21">
         <v>16</v>
       </c>
       <c r="C11" s="9"/>
       <c r="D11" s="24"/>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="21">
         <v>17</v>
       </c>
@@ -1638,7 +1652,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="21">
         <v>18</v>
       </c>
@@ -1649,7 +1663,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="43">
         <v>19</v>
       </c>
@@ -1660,7 +1674,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="30">
+    <row r="15" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="21">
         <v>20</v>
       </c>
@@ -1671,14 +1685,14 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="21">
         <v>21</v>
       </c>
       <c r="C16" s="6"/>
       <c r="D16" s="22"/>
     </row>
-    <row r="17" spans="2:4" ht="30">
+    <row r="17" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="21">
         <v>22</v>
       </c>
@@ -1689,21 +1703,21 @@
         <v>2.5</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="25">
         <v>23</v>
       </c>
       <c r="C18" s="46"/>
       <c r="D18" s="47"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="27">
         <v>24</v>
       </c>
       <c r="C19" s="28"/>
       <c r="D19" s="45"/>
     </row>
-    <row r="24" spans="2:4">
+    <row r="24" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C24" s="36" t="s">
         <v>14</v>
       </c>
@@ -1721,30 +1735,30 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="B3:D23"/>
   <sheetViews>
-    <sheetView workbookViewId="0" xr3:uid="{842E5F09-E766-5B8D-85AF-A39847EA96FD}">
+    <sheetView topLeftCell="A13" workbookViewId="0">
       <selection activeCell="E17" sqref="E17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.28515625" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="13.7109375" customWidth="1"/>
     <col min="3" max="3" width="34" customWidth="1"/>
     <col min="4" max="4" width="16" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:4">
+    <row r="3" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B3" s="1"/>
       <c r="C3" s="2" t="s">
         <v>31</v>
       </c>
       <c r="D3" s="1"/>
     </row>
-    <row r="4" spans="2:4">
+    <row r="4" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B4" s="1"/>
       <c r="C4" s="1"/>
       <c r="D4" s="1"/>
     </row>
-    <row r="5" spans="2:4" ht="30">
+    <row r="5" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B5" s="11" t="s">
         <v>1</v>
       </c>
@@ -1755,12 +1769,12 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="2:4">
+    <row r="6" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B6" s="3"/>
       <c r="C6" s="1"/>
       <c r="D6" s="51"/>
     </row>
-    <row r="7" spans="2:4">
+    <row r="7" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B7" s="5">
         <v>12</v>
       </c>
@@ -1771,7 +1785,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="8" spans="2:4">
+    <row r="8" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B8" s="5">
         <v>13</v>
       </c>
@@ -1782,7 +1796,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="9" spans="2:4" ht="30">
+    <row r="9" spans="2:4" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="5">
         <v>14</v>
       </c>
@@ -1793,7 +1807,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="2:4">
+    <row r="10" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B10" s="5">
         <v>15</v>
       </c>
@@ -1804,7 +1818,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="11" spans="2:4">
+    <row r="11" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B11" s="5">
         <v>16</v>
       </c>
@@ -1815,7 +1829,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="12" spans="2:4">
+    <row r="12" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B12" s="5">
         <v>17</v>
       </c>
@@ -1826,7 +1840,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="13" spans="2:4">
+    <row r="13" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B13" s="5">
         <v>18</v>
       </c>
@@ -1837,7 +1851,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="14" spans="2:4">
+    <row r="14" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B14" s="5">
         <v>19</v>
       </c>
@@ -1848,7 +1862,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="15" spans="2:4" ht="60">
+    <row r="15" spans="2:4" ht="60" x14ac:dyDescent="0.25">
       <c r="B15" s="5">
         <v>20</v>
       </c>
@@ -1859,14 +1873,14 @@
         <v>5</v>
       </c>
     </row>
-    <row r="16" spans="2:4">
+    <row r="16" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B16" s="5">
         <v>21</v>
       </c>
       <c r="C16" s="9"/>
       <c r="D16" s="52"/>
     </row>
-    <row r="17" spans="2:4" ht="45">
+    <row r="17" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B17" s="5">
         <v>22</v>
       </c>
@@ -1877,21 +1891,21 @@
         <v>4</v>
       </c>
     </row>
-    <row r="18" spans="2:4">
+    <row r="18" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B18" s="31">
         <v>23</v>
       </c>
       <c r="C18" s="29"/>
       <c r="D18" s="55"/>
     </row>
-    <row r="19" spans="2:4">
+    <row r="19" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B19" s="48">
         <v>24</v>
       </c>
       <c r="C19" s="41"/>
       <c r="D19" s="56"/>
     </row>
-    <row r="23" spans="2:4">
+    <row r="23" spans="2:4" x14ac:dyDescent="0.25">
       <c r="C23" t="s">
         <v>14</v>
       </c>

</xml_diff>